<commit_message>
rpg 2018 abstract organisation. epe 2081 synopsis intro + some sections are finished.
</commit_message>
<xml_diff>
--- a/Paper/EPE 2018/Plots.xlsx
+++ b/Paper/EPE 2018/Plots.xlsx
@@ -408,14 +408,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
-    <col min="3" max="3" width="45.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>